<commit_message>
Update DOmain Model - GLIK
Update DOmain Model - GLIK
</commit_message>
<xml_diff>
--- a/GLIK Domain Mapping.xlsx
+++ b/GLIK Domain Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toshiba\Documents\GitHub\GLIK-DM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFE4F68-2CD7-429D-A5CE-A6FE83C411D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0869C0F6-8BF0-4241-98E3-FCB8FBA6EE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{BC9BC3D9-6FF2-4CB4-96B2-33CE5FEE1DBD}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="462">
   <si>
     <t>Kode Fitur</t>
   </si>
@@ -1448,45 +1448,37 @@
     <t>17c. Dokumen Kewajiban</t>
   </si>
   <si>
-    <t>GPRM.Bank, GPRM.Pengurus, GPRM.Jaringan, BDL</t>
-  </si>
-  <si>
-    <t>GPRM.Bank, GPRM.Pengurus, BDL, RKABProfilBank, RKABPengurusProfilBank, RKABPeriodeProfilBank</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
-    <t>GPRM.Bank, GPRM.Pengurus, FiturUmum.Repository, BDL, RKABProfilBank, PembubaranBadanHukum, DocBadanHukum, MasterStatus</t>
-  </si>
-  <si>
-    <t>GPRM.Bank, GPRM.Pengurus, BDL, RKABProfilBank, RKABDebiturDanHapusBuku</t>
-  </si>
-  <si>
-    <t>GPRM.Bank, GPRM.Pengurus, RKABProfilBank, BDL, RKABPengurusProfilBank, RKABPeriodeProfilBank, HistoryGPDanTunjangan, TotalHistoryGPDanTunjangan</t>
-  </si>
-  <si>
-    <t>GPRM.Bank, GPRM.Pengurus, RKABProfilBank, BDL, RKABPengurusProfilBank, PembayaranKewajibanPegawai, TotalKewajibanDanPesangon</t>
-  </si>
-  <si>
-    <t>GPRM.Bank, GPRM.Pengurus, RKABProfilBank, BDL, RKABPengurusProfilBank, PembayaranKewajibanPegawai, TotalKewajibanDanPesangon, PerhitunganPesangon</t>
-  </si>
-  <si>
-    <r>
-      <t>GPRM.Bank, GPRM.Pengurus, B</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>DL, RKABProfilBank, RKABDebiturDanHapusBuku</t>
-    </r>
-  </si>
-  <si>
-    <t>GPRM.Bank, GPRM.Pengurus, FiturUmum.Repository, RKABProfilBank, BDL, RKABPengurusProfilBank, DocURLRepository, DocGLIK, DocDanaTalangan</t>
+    <t>GPRM.Bank, GPRM.Pengurus, BDL, RKABProfilBDL, RKABDebiturHapusBuku</t>
+  </si>
+  <si>
+    <t>GPRM.Bank, GPRM.Pengurus, FiturUmum.Repository, BDL, RKABProfilBDL, PembubaranBadanHukum, DocBadanHukum, MasterStatus</t>
+  </si>
+  <si>
+    <t>GPRM.Bank, GPRM.Pengurus, BDL, RKABProfilBDL, TenagaPendukung, TugasTenagaPendukung, MasterStatus</t>
+  </si>
+  <si>
+    <t>GPRM.Bank, GPRM.Pengurus, FiturUmum.Repository, BDL, RKABProfilBDL, KodeCabangBDL, TransaksiDataTalangan, JenisTransaksi, DocURLRepository, DocGLIK, DocTransaksiDanaTalangan, MasterStatus</t>
+  </si>
+  <si>
+    <t>GPRM.Bank, GPRM.Pengurus, GPRM.Jaringan, BDL, KodeCabangBDL</t>
+  </si>
+  <si>
+    <t>GPRM.Bank, GPRM.Pengurus, BDL, RKABProfilBDL, RKABPengurusBDL, ID_RKABPeriode</t>
+  </si>
+  <si>
+    <t>GPRM.Bank, GPRM.Pengurus, RKABProfilBDL, BDL, RKABPengurusBDL, ID_RKABPeriode, HistoryGPDanTunjangan, TotalGPDanTunjangan</t>
+  </si>
+  <si>
+    <t>GPRM.Bank, GPRM.Pengurus, RKABProfilBDL, BDL, RKABPengurusBDL, KewajibanPegawai, TotalKewajiban</t>
+  </si>
+  <si>
+    <t>GPRM.Bank, GPRM.Pengurus, RKABProfilBDL, BDL, RKABPengurusBDL, KewajibanPegawai, TotalKewajiban, PerhitunganPesangon, TotalPerhitunganPesangon</t>
+  </si>
+  <si>
+    <t>GPRM.Bank, GPRM.Pengurus, FiturUmum.Repository, BDL, RKABProfilBDL, RKABPengurusBDL, DocURLRepository, DocGLIK, DocDanaTalangan</t>
   </si>
 </sst>
 </file>
@@ -1599,7 +1591,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1634,6 +1626,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3876,7 +3877,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78815AC8-C3A4-42A1-9CFB-16EE2CA78EFD}">
   <dimension ref="B3:G72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -3884,9 +3885,9 @@
   <cols>
     <col min="1" max="1" width="8.7265625" style="1"/>
     <col min="2" max="2" width="3.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="58.81640625" style="16" customWidth="1"/>
     <col min="4" max="4" width="8.6328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="125.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="126.1796875" style="16" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
@@ -3908,60 +3909,60 @@
       <c r="B4" s="9">
         <v>1</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="15" t="s">
         <v>382</v>
       </c>
       <c r="D4" s="9"/>
-      <c r="E4" s="8" t="s">
-        <v>451</v>
+      <c r="E4" s="15" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="9">
         <v>2</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="15" t="s">
         <v>383</v>
       </c>
       <c r="D5" s="9"/>
-      <c r="E5" s="8" t="s">
-        <v>451</v>
+      <c r="E5" s="15" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="9">
         <v>3</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="15" t="s">
         <v>384</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="8" t="s">
-        <v>452</v>
+      <c r="E6" s="15" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" s="9">
         <v>4</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="15" t="s">
         <v>385</v>
       </c>
       <c r="D7" s="9"/>
-      <c r="E7" s="8" t="s">
-        <v>459</v>
+      <c r="E7" s="15" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="9">
         <v>5</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="15" t="s">
         <v>386</v>
       </c>
       <c r="D8" s="9"/>
-      <c r="E8" s="8" t="s">
-        <v>455</v>
+      <c r="E8" s="15" t="s">
+        <v>452</v>
       </c>
       <c r="G8" s="10"/>
     </row>
@@ -3969,665 +3970,671 @@
       <c r="B9" s="9">
         <v>6</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="15" t="s">
         <v>387</v>
       </c>
       <c r="D9" s="9"/>
-      <c r="E9" s="8" t="s">
-        <v>455</v>
+      <c r="E9" s="15" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" s="9">
         <v>7</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="15" t="s">
         <v>388</v>
       </c>
       <c r="D10" s="9"/>
-      <c r="E10" s="8" t="s">
-        <v>453</v>
+      <c r="E10" s="15" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" s="9">
         <v>8</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="15" t="s">
         <v>389</v>
       </c>
       <c r="D11" s="9"/>
-      <c r="E11" s="8" t="s">
-        <v>454</v>
+      <c r="E11" s="15" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" s="9">
         <v>9</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="15" t="s">
         <v>390</v>
       </c>
       <c r="D12" s="9"/>
-      <c r="E12" s="8" t="s">
-        <v>454</v>
+      <c r="E12" s="15" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B13" s="9">
         <v>10</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="15" t="s">
         <v>391</v>
       </c>
       <c r="D13" s="9"/>
-      <c r="E13" s="8" t="s">
-        <v>454</v>
+      <c r="E13" s="15" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14" s="9">
         <v>11</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="15" t="s">
         <v>392</v>
       </c>
       <c r="D14" s="9"/>
-      <c r="E14" s="8" t="s">
-        <v>454</v>
+      <c r="E14" s="15" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B15" s="9">
         <v>12</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="15" t="s">
         <v>393</v>
       </c>
       <c r="D15" s="9"/>
-      <c r="E15" s="8" t="s">
-        <v>456</v>
+      <c r="E15" s="15" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B16" s="9">
         <v>13</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="15" t="s">
         <v>394</v>
       </c>
       <c r="D16" s="9"/>
-      <c r="E16" s="8" t="s">
-        <v>456</v>
+      <c r="E16" s="15" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" s="9">
         <v>14</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="15" t="s">
         <v>395</v>
       </c>
       <c r="D17" s="9"/>
-      <c r="E17" s="8" t="s">
-        <v>457</v>
+      <c r="E17" s="15" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" s="9">
         <v>15</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="15" t="s">
         <v>396</v>
       </c>
       <c r="D18" s="9"/>
-      <c r="E18" s="8" t="s">
-        <v>458</v>
+      <c r="E18" s="15" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B19" s="9">
         <v>16</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="15" t="s">
         <v>397</v>
       </c>
       <c r="D19" s="9"/>
-      <c r="E19" s="8" t="s">
-        <v>458</v>
+      <c r="E19" s="15" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="9">
         <v>17</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="15" t="s">
         <v>398</v>
       </c>
       <c r="D20" s="9"/>
-      <c r="E20" s="8" t="s">
-        <v>460</v>
+      <c r="E20" s="15" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B21" s="9">
         <v>18</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="15" t="s">
         <v>399</v>
       </c>
       <c r="D21" s="9"/>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="E21" s="15" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="26" x14ac:dyDescent="0.3">
       <c r="B22" s="9">
         <v>19</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="15" t="s">
         <v>400</v>
       </c>
       <c r="D22" s="9"/>
-      <c r="E22" s="8"/>
+      <c r="E22" s="17" t="s">
+        <v>455</v>
+      </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B23" s="9">
         <v>20</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="15" t="s">
         <v>401</v>
       </c>
       <c r="D23" s="9"/>
-      <c r="E23" s="8"/>
+      <c r="E23" s="15" t="s">
+        <v>454</v>
+      </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B24" s="9">
         <v>21</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="15" t="s">
         <v>402</v>
       </c>
       <c r="D24" s="9"/>
-      <c r="E24" s="8"/>
+      <c r="E24" s="15"/>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B25" s="9">
         <v>22</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="C25" s="15" t="s">
         <v>403</v>
       </c>
       <c r="D25" s="9"/>
-      <c r="E25" s="8"/>
+      <c r="E25" s="15"/>
     </row>
     <row r="26" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B26" s="9">
         <v>23</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="15" t="s">
         <v>404</v>
       </c>
       <c r="D26" s="9"/>
-      <c r="E26" s="8"/>
+      <c r="E26" s="15"/>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B27" s="9">
         <v>24</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="15" t="s">
         <v>405</v>
       </c>
       <c r="D27" s="9"/>
-      <c r="E27" s="8"/>
+      <c r="E27" s="15"/>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B28" s="9">
         <v>25</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="15" t="s">
         <v>406</v>
       </c>
       <c r="D28" s="9"/>
-      <c r="E28" s="8"/>
+      <c r="E28" s="15"/>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B29" s="9">
         <v>26</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="15" t="s">
         <v>407</v>
       </c>
       <c r="D29" s="9"/>
-      <c r="E29" s="8"/>
+      <c r="E29" s="15"/>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B30" s="9">
         <v>27</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="15" t="s">
         <v>408</v>
       </c>
       <c r="D30" s="9"/>
-      <c r="E30" s="8"/>
+      <c r="E30" s="15"/>
     </row>
     <row r="31" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B31" s="9">
         <v>28</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="15" t="s">
         <v>409</v>
       </c>
       <c r="D31" s="9"/>
-      <c r="E31" s="8"/>
+      <c r="E31" s="15"/>
     </row>
     <row r="32" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B32" s="9">
         <v>29</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="15" t="s">
         <v>410</v>
       </c>
       <c r="D32" s="9"/>
-      <c r="E32" s="8"/>
+      <c r="E32" s="15"/>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B33" s="9">
         <v>30</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="C33" s="15" t="s">
         <v>411</v>
       </c>
       <c r="D33" s="9"/>
-      <c r="E33" s="8"/>
+      <c r="E33" s="15"/>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B34" s="9">
         <v>31</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="15" t="s">
         <v>412</v>
       </c>
       <c r="D34" s="9"/>
-      <c r="E34" s="8"/>
+      <c r="E34" s="15"/>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B35" s="9">
         <v>32</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="15" t="s">
         <v>413</v>
       </c>
       <c r="D35" s="9"/>
-      <c r="E35" s="8"/>
+      <c r="E35" s="15"/>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B36" s="9">
         <v>33</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="15" t="s">
         <v>414</v>
       </c>
       <c r="D36" s="9"/>
-      <c r="E36" s="8"/>
+      <c r="E36" s="15"/>
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B37" s="9">
         <v>34</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="C37" s="15" t="s">
         <v>415</v>
       </c>
       <c r="D37" s="9"/>
-      <c r="E37" s="8"/>
+      <c r="E37" s="15"/>
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B38" s="9">
         <v>35</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="C38" s="15" t="s">
         <v>416</v>
       </c>
       <c r="D38" s="9"/>
-      <c r="E38" s="8"/>
+      <c r="E38" s="15"/>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B39" s="9">
         <v>36</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="C39" s="15" t="s">
         <v>417</v>
       </c>
       <c r="D39" s="9"/>
-      <c r="E39" s="8"/>
+      <c r="E39" s="15"/>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B40" s="9">
         <v>37</v>
       </c>
-      <c r="C40" s="8" t="s">
+      <c r="C40" s="15" t="s">
         <v>418</v>
       </c>
       <c r="D40" s="9"/>
-      <c r="E40" s="8"/>
+      <c r="E40" s="15"/>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B41" s="9">
         <v>38</v>
       </c>
-      <c r="C41" s="8" t="s">
+      <c r="C41" s="15" t="s">
         <v>419</v>
       </c>
       <c r="D41" s="9"/>
-      <c r="E41" s="8"/>
+      <c r="E41" s="15"/>
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B42" s="9">
         <v>39</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="C42" s="15" t="s">
         <v>420</v>
       </c>
       <c r="D42" s="9"/>
-      <c r="E42" s="8"/>
+      <c r="E42" s="15"/>
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B43" s="9">
         <v>40</v>
       </c>
-      <c r="C43" s="8" t="s">
+      <c r="C43" s="15" t="s">
         <v>421</v>
       </c>
       <c r="D43" s="9"/>
-      <c r="E43" s="8"/>
+      <c r="E43" s="15"/>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B44" s="9">
         <v>41</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="C44" s="15" t="s">
         <v>422</v>
       </c>
       <c r="D44" s="9"/>
-      <c r="E44" s="8"/>
+      <c r="E44" s="15"/>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B45" s="9">
         <v>42</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C45" s="15" t="s">
         <v>423</v>
       </c>
       <c r="D45" s="9"/>
-      <c r="E45" s="8"/>
+      <c r="E45" s="15"/>
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B46" s="9">
         <v>43</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="15" t="s">
         <v>424</v>
       </c>
       <c r="D46" s="9"/>
-      <c r="E46" s="8"/>
+      <c r="E46" s="15"/>
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B47" s="9">
         <v>44</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="C47" s="15" t="s">
         <v>425</v>
       </c>
       <c r="D47" s="9"/>
-      <c r="E47" s="8"/>
+      <c r="E47" s="15"/>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B48" s="9">
         <v>45</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="C48" s="15" t="s">
         <v>426</v>
       </c>
       <c r="D48" s="9"/>
-      <c r="E48" s="8"/>
+      <c r="E48" s="15"/>
     </row>
     <row r="49" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B49" s="9">
         <v>46</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="C49" s="15" t="s">
         <v>427</v>
       </c>
       <c r="D49" s="9"/>
-      <c r="E49" s="8"/>
+      <c r="E49" s="15"/>
     </row>
     <row r="50" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B50" s="9">
         <v>47</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="C50" s="15" t="s">
         <v>428</v>
       </c>
       <c r="D50" s="9"/>
-      <c r="E50" s="8"/>
+      <c r="E50" s="15"/>
     </row>
     <row r="51" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B51" s="9">
         <v>48</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="C51" s="15" t="s">
         <v>429</v>
       </c>
       <c r="D51" s="9"/>
-      <c r="E51" s="8"/>
+      <c r="E51" s="15"/>
     </row>
     <row r="52" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B52" s="9">
         <v>49</v>
       </c>
-      <c r="C52" s="8" t="s">
+      <c r="C52" s="15" t="s">
         <v>430</v>
       </c>
       <c r="D52" s="9"/>
-      <c r="E52" s="8"/>
+      <c r="E52" s="15"/>
     </row>
     <row r="53" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B53" s="9">
         <v>50</v>
       </c>
-      <c r="C53" s="8" t="s">
+      <c r="C53" s="15" t="s">
         <v>431</v>
       </c>
       <c r="D53" s="9"/>
-      <c r="E53" s="8"/>
+      <c r="E53" s="15"/>
     </row>
     <row r="54" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B54" s="9">
         <v>51</v>
       </c>
-      <c r="C54" s="8" t="s">
+      <c r="C54" s="15" t="s">
         <v>432</v>
       </c>
       <c r="D54" s="9"/>
-      <c r="E54" s="8"/>
+      <c r="E54" s="15"/>
     </row>
     <row r="55" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B55" s="9">
         <v>52</v>
       </c>
-      <c r="C55" s="8" t="s">
+      <c r="C55" s="15" t="s">
         <v>433</v>
       </c>
       <c r="D55" s="9"/>
-      <c r="E55" s="8"/>
+      <c r="E55" s="15"/>
     </row>
     <row r="56" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B56" s="9">
         <v>53</v>
       </c>
-      <c r="C56" s="8" t="s">
+      <c r="C56" s="15" t="s">
         <v>434</v>
       </c>
       <c r="D56" s="9"/>
-      <c r="E56" s="8"/>
+      <c r="E56" s="15"/>
     </row>
     <row r="57" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B57" s="9">
         <v>54</v>
       </c>
-      <c r="C57" s="8" t="s">
+      <c r="C57" s="15" t="s">
         <v>435</v>
       </c>
       <c r="D57" s="9"/>
-      <c r="E57" s="8"/>
+      <c r="E57" s="15"/>
     </row>
     <row r="58" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B58" s="9">
         <v>55</v>
       </c>
-      <c r="C58" s="8" t="s">
+      <c r="C58" s="15" t="s">
         <v>436</v>
       </c>
       <c r="D58" s="9"/>
-      <c r="E58" s="8"/>
+      <c r="E58" s="15"/>
     </row>
     <row r="59" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B59" s="9">
         <v>56</v>
       </c>
-      <c r="C59" s="8" t="s">
+      <c r="C59" s="15" t="s">
         <v>437</v>
       </c>
       <c r="D59" s="9"/>
-      <c r="E59" s="8"/>
+      <c r="E59" s="15"/>
     </row>
     <row r="60" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B60" s="9">
         <v>57</v>
       </c>
-      <c r="C60" s="8" t="s">
+      <c r="C60" s="15" t="s">
         <v>438</v>
       </c>
       <c r="D60" s="9"/>
-      <c r="E60" s="8"/>
+      <c r="E60" s="15"/>
     </row>
     <row r="61" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B61" s="9">
         <v>58</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="C61" s="15" t="s">
         <v>439</v>
       </c>
       <c r="D61" s="9"/>
-      <c r="E61" s="8"/>
+      <c r="E61" s="15"/>
     </row>
     <row r="62" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B62" s="9">
         <v>59</v>
       </c>
-      <c r="C62" s="8" t="s">
+      <c r="C62" s="15" t="s">
         <v>440</v>
       </c>
       <c r="D62" s="9"/>
-      <c r="E62" s="8"/>
+      <c r="E62" s="15"/>
     </row>
     <row r="63" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B63" s="9">
         <v>60</v>
       </c>
-      <c r="C63" s="8" t="s">
+      <c r="C63" s="15" t="s">
         <v>441</v>
       </c>
       <c r="D63" s="9"/>
-      <c r="E63" s="8"/>
+      <c r="E63" s="15"/>
     </row>
     <row r="64" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B64" s="9">
         <v>61</v>
       </c>
-      <c r="C64" s="8" t="s">
+      <c r="C64" s="15" t="s">
         <v>442</v>
       </c>
       <c r="D64" s="9"/>
-      <c r="E64" s="8"/>
+      <c r="E64" s="15"/>
     </row>
     <row r="65" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B65" s="9">
         <v>62</v>
       </c>
-      <c r="C65" s="8" t="s">
+      <c r="C65" s="15" t="s">
         <v>443</v>
       </c>
       <c r="D65" s="9"/>
-      <c r="E65" s="8"/>
+      <c r="E65" s="15"/>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B66" s="9">
         <v>63</v>
       </c>
-      <c r="C66" s="8" t="s">
+      <c r="C66" s="15" t="s">
         <v>444</v>
       </c>
       <c r="D66" s="9"/>
-      <c r="E66" s="8"/>
+      <c r="E66" s="15"/>
     </row>
     <row r="67" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B67" s="9">
         <v>64</v>
       </c>
-      <c r="C67" s="8" t="s">
+      <c r="C67" s="15" t="s">
         <v>445</v>
       </c>
       <c r="D67" s="9"/>
-      <c r="E67" s="8"/>
+      <c r="E67" s="15"/>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B68" s="9">
         <v>65</v>
       </c>
-      <c r="C68" s="8" t="s">
+      <c r="C68" s="15" t="s">
         <v>446</v>
       </c>
       <c r="D68" s="9"/>
-      <c r="E68" s="8"/>
+      <c r="E68" s="15"/>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B69" s="9">
         <v>66</v>
       </c>
-      <c r="C69" s="8" t="s">
+      <c r="C69" s="15" t="s">
         <v>447</v>
       </c>
       <c r="D69" s="9"/>
-      <c r="E69" s="8"/>
+      <c r="E69" s="15"/>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B70" s="9">
         <v>67</v>
       </c>
-      <c r="C70" s="8" t="s">
+      <c r="C70" s="15" t="s">
         <v>448</v>
       </c>
       <c r="D70" s="9"/>
-      <c r="E70" s="8"/>
+      <c r="E70" s="15"/>
     </row>
     <row r="71" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B71" s="9">
         <v>68</v>
       </c>
-      <c r="C71" s="8" t="s">
+      <c r="C71" s="15" t="s">
         <v>449</v>
       </c>
       <c r="D71" s="9"/>
-      <c r="E71" s="8"/>
+      <c r="E71" s="15"/>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B72" s="9">
         <v>69</v>
       </c>
-      <c r="C72" s="8" t="s">
+      <c r="C72" s="15" t="s">
         <v>450</v>
       </c>
       <c r="D72" s="9"/>
-      <c r="E72" s="8"/>
+      <c r="E72" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>